<commit_message>
Adds teardrops and polygons that were missing after changes
</commit_message>
<xml_diff>
--- a/Project Outputs for ZYNQ_IPMC/revB1/BOM/Bill of Materials-ZYNQ_IPMC.xlsx
+++ b/Project Outputs for ZYNQ_IPMC/revB1/BOM/Bill of Materials-ZYNQ_IPMC.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7579A0F9-D6C5-4C30-BC57-B67FE1CDA2CE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{252BB4A7-E4A5-4F5C-BDF8-506DC8AC5FCB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="735" windowWidth="18225" windowHeight="11422" xr2:uid="{B91997FF-6278-4A52-A137-7C9C92519164}"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="18225" windowHeight="11422" xr2:uid="{5350EEB0-BCC5-4A7E-8585-314380F33A4B}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-ZYNQ_IPMC" sheetId="1" r:id="rId1"/>
@@ -1347,7 +1347,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7B0F994-04DA-44D4-B810-21BFACA46D94}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E9E9ED7-B6EF-407C-A452-8C3E8EC004D1}">
   <dimension ref="A1:M60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>